<commit_message>
Revised excel workbooks and CSV data files
</commit_message>
<xml_diff>
--- a/Supp2_WHO-growth-reference-tables_2006.xlsx
+++ b/Supp2_WHO-growth-reference-tables_2006.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kates\Box\CANDASA (Shared Files)\Outputs\GhTzMw_SoftwareTools\Nutrient Requirements - DRIs + WHO growth charts\Gates Open Research Article\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/771c65effd2904ee/Documents/GitHub/Nutrient-Requirements-Software-Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD49221-1C79-4B03-9DE2-3EF32F30E1AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{6CD49221-1C79-4B03-9DE2-3EF32F30E1AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BB2FFE47-F318-45F4-9CA8-C6485F31FA3C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="856" xr2:uid="{27546790-665F-4F27-8989-9999E4E1E090}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="856" xr2:uid="{27546790-665F-4F27-8989-9999E4E1E090}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="14" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="124">
   <si>
     <t>Month</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>Length/Height-for-Age Percentiles, 0-5, Girls</t>
-  </si>
-  <si>
-    <t>Indicator</t>
   </si>
   <si>
     <t>kg/month</t>
@@ -526,9 +523,6 @@
     </r>
   </si>
   <si>
-    <t>Dataset</t>
-  </si>
-  <si>
     <t xml:space="preserve">Notes: </t>
   </si>
   <si>
@@ -538,55 +532,22 @@
     <t>It calculates reference weights and heights, protein, and energy requirements using the WHO growth charts as the reference anthropometry parameters for the Dietary Reference Intakes age and sex groups contained in Supplement 1.</t>
   </si>
   <si>
-    <t>2_WHOGrowthCharts_EnergyEER</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_ProteinEAR</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_MedianWeightHeightMonth0-19</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_WeightsHeightsbyDRIGroup</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_WFA0-5Boys</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_LHFA0-5Boys</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_BMI5-19Boys</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_HFA5-19Boys</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_MedianWeightHeightYear5-19</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_WFA0-5Girls</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_LHFA0-5Girls</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_BMI5-19Girls</t>
-  </si>
-  <si>
-    <t>2_WHOGrowthCharts_HFA5-19Girls</t>
-  </si>
-  <si>
     <t>BMI-for-Age, 5-19, Girls</t>
   </si>
   <si>
     <t>Height-for-Age, 5-19, Girls</t>
   </si>
   <si>
-    <t>Supplement 2 contains 14 datasets</t>
+    <t>Sheets</t>
   </si>
   <si>
-    <t>2_WHOGrowthCharts_Notes</t>
+    <t>Supplement 2 contains 14 sheets</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Indicator/Description</t>
   </si>
 </sst>
 </file>
@@ -782,18 +743,6 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -808,6 +757,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1134,7 +1095,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,8 +1107,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>115</v>
+      <c r="A1" s="36" t="s">
+        <v>114</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1156,12 +1117,12 @@
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="29"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
@@ -1170,49 +1131,49 @@
       <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="A4" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="A5" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="A6" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+        <v>121</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
@@ -1226,180 +1187,182 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="35" t="s">
+    <row r="9" spans="1:8" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33">
+        <v>1</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
+        <v>2</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
+        <v>3</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33">
+        <v>4</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33">
+        <v>5</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-    </row>
-    <row r="11" spans="1:8" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="38" t="s">
+    </row>
+    <row r="15" spans="1:8" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33">
+        <v>6</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33">
+        <v>7</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33">
+        <v>8</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="38" t="s">
+    <row r="18" spans="1:4" s="33" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="33">
+        <v>9</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19" s="38" t="s">
+    <row r="19" spans="1:4" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33">
+        <v>10</v>
+      </c>
+      <c r="B19" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33">
+        <v>11</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33">
+        <v>12</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="33" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="33">
+        <v>13</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="B23" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>67</v>
+    <row r="23" spans="1:4" s="33" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33">
+        <v>14</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1413,20 +1376,20 @@
       <c r="B28" s="6"/>
     </row>
     <row r="29" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
+      <c r="A29" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
     </row>
     <row r="30" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
+      <c r="A30" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
     </row>
     <row r="31" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
@@ -1436,22 +1399,22 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1494,23 +1457,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H1" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
+      <c r="H1" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -13032,19 +12995,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G1" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
+      <c r="G1" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -16360,23 +16323,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H1" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
+      <c r="H1" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -20621,19 +20584,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="G1" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
+      <c r="G1" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -29620,23 +29583,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H1" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
+      <c r="H1" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -41163,13 +41126,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>34</v>
@@ -41184,10 +41147,10 @@
         <v>55</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -41971,13 +41934,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>34</v>
@@ -41986,28 +41949,28 @@
         <v>35</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="L1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -42042,7 +42005,7 @@
         <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L2" t="s">
         <v>43</v>
@@ -42083,7 +42046,7 @@
         <v>669.6</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L3" s="5">
         <f>J3</f>
@@ -42125,7 +42088,7 @@
         <v>965.75</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" ref="L4:L67" si="0">J4</f>
@@ -42170,7 +42133,7 @@
         <v>1277.25</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L5" s="5">
         <f>J5</f>
@@ -42215,7 +42178,7 @@
         <v>1246.1000000000001</v>
       </c>
       <c r="K6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="0"/>
@@ -42260,7 +42223,7 @@
         <v>1443.3312339098061</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="0"/>
@@ -42305,7 +42268,7 @@
         <v>1308.6378278870002</v>
       </c>
       <c r="K8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="0"/>
@@ -42350,7 +42313,7 @@
         <v>1860.235493668742</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="0"/>
@@ -42395,7 +42358,7 @@
         <v>2638.4336192739597</v>
       </c>
       <c r="K10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="0"/>
@@ -42440,7 +42403,7 @@
         <v>2650.5780195074303</v>
       </c>
       <c r="K11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="0"/>
@@ -42485,7 +42448,7 @@
         <v>2291.1698724152229</v>
       </c>
       <c r="K12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="0"/>
@@ -42530,7 +42493,7 @@
         <v>2100.569872415223</v>
       </c>
       <c r="K13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="0"/>
@@ -42575,7 +42538,7 @@
         <v>1962.3848724152231</v>
       </c>
       <c r="K14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="0"/>
@@ -42620,7 +42583,7 @@
         <v>1649.3944265350001</v>
       </c>
       <c r="K15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="0"/>
@@ -42665,7 +42628,7 @@
         <v>1834.3845048322</v>
       </c>
       <c r="K16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="0"/>
@@ -42710,7 +42673,7 @@
         <v>1994.5994544417399</v>
       </c>
       <c r="K17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L17" s="5">
         <f t="shared" si="0"/>
@@ -42755,7 +42718,7 @@
         <v>1792.5233443116799</v>
       </c>
       <c r="K18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" si="0"/>
@@ -42800,7 +42763,7 @@
         <v>1654.3233443116799</v>
       </c>
       <c r="K19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L19" s="5">
         <f t="shared" si="0"/>
@@ -42845,7 +42808,7 @@
         <v>1554.1283443116799</v>
       </c>
       <c r="K20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L20" s="5">
         <f t="shared" si="0"/>
@@ -42890,7 +42853,7 @@
         <v>2311.1108548321999</v>
       </c>
       <c r="K21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" si="0"/>
@@ -42935,7 +42898,7 @@
         <v>2458.6194544417399</v>
       </c>
       <c r="K22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L22" s="5">
         <f t="shared" si="0"/>
@@ -42980,7 +42943,7 @@
         <v>2256.5433443116799</v>
       </c>
       <c r="K23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="0"/>
@@ -43025,7 +42988,7 @@
         <v>2091.744884093675</v>
       </c>
       <c r="K24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L24" s="5">
         <f t="shared" si="0"/>
@@ -43070,7 +43033,7 @@
         <v>2233.0833443116799</v>
       </c>
       <c r="K25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L25" s="5">
         <f t="shared" si="0"/>
@@ -43115,7 +43078,7 @@
         <v>2122.5233443116799</v>
       </c>
       <c r="K26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L26" s="5">
         <f t="shared" si="0"/>
@@ -43157,7 +43120,7 @@
         <v>43</v>
       </c>
       <c r="K27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L27" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43199,7 +43162,7 @@
         <v>669.6</v>
       </c>
       <c r="K28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L28" s="5">
         <f t="shared" si="0"/>
@@ -43241,7 +43204,7 @@
         <v>965.75</v>
       </c>
       <c r="K29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L29" s="5">
         <f t="shared" si="0"/>
@@ -43286,7 +43249,7 @@
         <v>1277.25</v>
       </c>
       <c r="K30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L30" s="5">
         <f t="shared" si="0"/>
@@ -43331,7 +43294,7 @@
         <v>1246.1000000000001</v>
       </c>
       <c r="K31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L31" s="5">
         <f t="shared" si="0"/>
@@ -43376,7 +43339,7 @@
         <v>1667.7412943180807</v>
       </c>
       <c r="K32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L32" s="5">
         <f t="shared" si="0"/>
@@ -43421,7 +43384,7 @@
         <v>1525.93988034892</v>
       </c>
       <c r="K33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L33" s="5">
         <f t="shared" si="0"/>
@@ -43466,7 +43429,7 @@
         <v>2596.0261417693646</v>
       </c>
       <c r="K34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L34" s="5">
         <f t="shared" si="0"/>
@@ -43511,7 +43474,7 @@
         <v>3700.5337050561479</v>
       </c>
       <c r="K35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L35" s="5">
         <f t="shared" si="0"/>
@@ -43556,7 +43519,7 @@
         <v>2895.0049516532481</v>
       </c>
       <c r="K36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L36" s="5">
         <f t="shared" si="0"/>
@@ -43601,7 +43564,7 @@
         <v>2512.8347083808976</v>
       </c>
       <c r="K37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L37" s="5">
         <f t="shared" si="0"/>
@@ -43646,7 +43609,7 @@
         <v>2322.2347083808977</v>
       </c>
       <c r="K38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L38" s="5">
         <f t="shared" si="0"/>
@@ -43691,7 +43654,7 @@
         <v>2184.0497083808978</v>
       </c>
       <c r="K39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L39" s="5">
         <f t="shared" si="0"/>
@@ -43736,7 +43699,7 @@
         <v>1945.8575347806</v>
       </c>
       <c r="K40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L40" s="5">
         <f t="shared" si="0"/>
@@ -43781,7 +43744,7 @@
         <v>2185.086025605352</v>
       </c>
       <c r="K41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L41" s="5">
         <f t="shared" si="0"/>
@@ -43826,7 +43789,7 @@
         <v>2211.786788974749</v>
       </c>
       <c r="K42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L42" s="5">
         <f t="shared" si="0"/>
@@ -43871,7 +43834,7 @@
         <v>1998.7287456290817</v>
       </c>
       <c r="K43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L43" s="5">
         <f t="shared" si="0"/>
@@ -43916,7 +43879,7 @@
         <v>1860.5287456290816</v>
       </c>
       <c r="K44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L44" s="5">
         <f t="shared" si="0"/>
@@ -43961,7 +43924,7 @@
         <v>1760.3337456290817</v>
       </c>
       <c r="K45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L45" s="5">
         <f t="shared" si="0"/>
@@ -44006,7 +43969,7 @@
         <v>2590.5441574120641</v>
       </c>
       <c r="K46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L46" s="5">
         <f t="shared" si="0"/>
@@ -44051,7 +44014,7 @@
         <v>2690.689188974749</v>
       </c>
       <c r="K47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L47" s="5">
         <f t="shared" si="0"/>
@@ -44096,7 +44059,7 @@
         <v>2477.6311456290819</v>
       </c>
       <c r="K48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L48" s="5">
         <f t="shared" si="0"/>
@@ -44141,7 +44104,7 @@
         <v>2346.0542701849163</v>
       </c>
       <c r="K49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L49" s="5">
         <f t="shared" si="0"/>
@@ -44186,7 +44149,7 @@
         <v>2439.2887456290819</v>
       </c>
       <c r="K50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L50" s="5">
         <f t="shared" si="0"/>
@@ -44231,7 +44194,7 @@
         <v>2328.7287456290815</v>
       </c>
       <c r="K51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L51" s="5">
         <f t="shared" si="0"/>
@@ -44273,7 +44236,7 @@
         <v>43</v>
       </c>
       <c r="K52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L52" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44315,7 +44278,7 @@
         <v>669.6</v>
       </c>
       <c r="K53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L53" s="5">
         <f t="shared" si="0"/>
@@ -44357,7 +44320,7 @@
         <v>965.75</v>
       </c>
       <c r="K54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L54" s="5">
         <f t="shared" si="0"/>
@@ -44402,7 +44365,7 @@
         <v>1277.25</v>
       </c>
       <c r="K55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L55" s="5">
         <f t="shared" si="0"/>
@@ -44447,7 +44410,7 @@
         <v>1246.1000000000001</v>
       </c>
       <c r="K56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L56" s="5">
         <f t="shared" si="0"/>
@@ -44492,7 +44455,7 @@
         <v>1892.1513547263557</v>
       </c>
       <c r="K57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L57" s="5">
         <f t="shared" si="0"/>
@@ -44537,7 +44500,7 @@
         <v>1729.6605545319703</v>
       </c>
       <c r="K58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L58" s="5">
         <f t="shared" si="0"/>
@@ -44582,7 +44545,7 @@
         <v>2497.9207220226149</v>
       </c>
       <c r="K59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L59" s="5">
         <f t="shared" si="0"/>
@@ -44627,7 +44590,7 @@
         <v>3558.920360285189</v>
       </c>
       <c r="K60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L60" s="5">
         <f t="shared" si="0"/>
@@ -44672,7 +44635,7 @@
         <v>3206.0937743842878</v>
       </c>
       <c r="K61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L61" s="5">
         <f t="shared" si="0"/>
@@ -44717,7 +44680,7 @@
         <v>2794.9535905190287</v>
       </c>
       <c r="K62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L62" s="5">
         <f t="shared" si="0"/>
@@ -44762,7 +44725,7 @@
         <v>2604.3535905190288</v>
       </c>
       <c r="K63" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L63" s="5">
         <f t="shared" si="0"/>
@@ -44807,7 +44770,7 @@
         <v>2466.1685905190288</v>
       </c>
       <c r="K64" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L64" s="5">
         <f t="shared" si="0"/>
@@ -44852,7 +44815,7 @@
         <v>2223.7916987608501</v>
       </c>
       <c r="K65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L65" s="5">
         <f t="shared" si="0"/>
@@ -44897,7 +44860,7 @@
         <v>2513.8687013301824</v>
       </c>
       <c r="K66" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L66" s="5">
         <f t="shared" si="0"/>
@@ -44942,7 +44905,7 @@
         <v>2483.2709571410096</v>
       </c>
       <c r="K67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L67" s="5">
         <f t="shared" si="0"/>
@@ -44987,7 +44950,7 @@
         <v>2256.4854972758335</v>
       </c>
       <c r="K68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L68" s="5">
         <f t="shared" ref="L68:L101" si="3">J68</f>
@@ -45032,7 +44995,7 @@
         <v>2118.2854972758337</v>
       </c>
       <c r="K69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L69" s="5">
         <f t="shared" si="3"/>
@@ -45077,7 +45040,7 @@
         <v>2018.0904972758335</v>
       </c>
       <c r="K70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L70" s="5">
         <f t="shared" si="3"/>
@@ -45122,7 +45085,7 @@
         <v>2939.8357856368939</v>
       </c>
       <c r="K71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L71" s="5">
         <f t="shared" si="3"/>
@@ -45167,7 +45130,7 @@
         <v>2980.7763571410096</v>
       </c>
       <c r="K72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L72" s="5">
         <f t="shared" si="3"/>
@@ -45212,7 +45175,7 @@
         <v>2753.9908972758335</v>
       </c>
       <c r="K73" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L73" s="5">
         <f t="shared" si="3"/>
@@ -45257,7 +45220,7 @@
         <v>2663.941002798967</v>
       </c>
       <c r="K74" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L74" s="5">
         <f t="shared" si="3"/>
@@ -45302,7 +45265,7 @@
         <v>2697.0454972758334</v>
       </c>
       <c r="K75" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L75" s="5">
         <f t="shared" si="3"/>
@@ -45347,7 +45310,7 @@
         <v>2586.4854972758335</v>
       </c>
       <c r="K76" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L76" s="5">
         <f t="shared" si="3"/>
@@ -45389,7 +45352,7 @@
         <v>43</v>
       </c>
       <c r="K77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L77" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45431,7 +45394,7 @@
         <v>669.6</v>
       </c>
       <c r="K78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L78" s="5">
         <f t="shared" si="3"/>
@@ -45473,7 +45436,7 @@
         <v>965.75</v>
       </c>
       <c r="K79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L79" s="5">
         <f t="shared" si="3"/>
@@ -45518,7 +45481,7 @@
         <v>1277.25</v>
       </c>
       <c r="K80" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L80" s="5">
         <f t="shared" si="3"/>
@@ -45563,7 +45526,7 @@
         <v>1246.1000000000001</v>
       </c>
       <c r="K81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L81" s="5">
         <f t="shared" si="3"/>
@@ -45608,7 +45571,7 @@
         <v>2168.3483521519247</v>
       </c>
       <c r="K82" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L82" s="5">
         <f t="shared" si="3"/>
@@ -45653,7 +45616,7 @@
         <v>2069.1950115037203</v>
       </c>
       <c r="K83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L83" s="5">
         <f t="shared" si="3"/>
@@ -45698,7 +45661,7 @@
         <v>2890.3424010096137</v>
       </c>
       <c r="K84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L84" s="5">
         <f t="shared" si="3"/>
@@ -45743,7 +45706,7 @@
         <v>4125.3737393690235</v>
       </c>
       <c r="K85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L85" s="5">
         <f t="shared" si="3"/>
@@ -45788,7 +45751,7 @@
         <v>3717.1682688709971</v>
       </c>
       <c r="K86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L86" s="5">
         <f t="shared" si="3"/>
@@ -45833,7 +45796,7 @@
         <v>3258.4346111745299</v>
       </c>
       <c r="K87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L87" s="5">
         <f t="shared" si="3"/>
@@ -45878,7 +45841,7 @@
         <v>3067.83461117453</v>
       </c>
       <c r="K88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L88" s="5">
         <f t="shared" si="3"/>
@@ -45923,7 +45886,7 @@
         <v>2929.64961117453</v>
       </c>
       <c r="K89" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L89" s="5">
         <f t="shared" si="3"/>
@@ -45968,7 +45931,7 @@
         <v>2687.0153053946001</v>
       </c>
       <c r="K90" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L90" s="5">
         <f t="shared" si="3"/>
@@ -46013,7 +45976,7 @@
         <v>3061.8398275382324</v>
       </c>
       <c r="K91" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L91" s="5">
         <f t="shared" si="3"/>
@@ -46058,7 +46021,7 @@
         <v>2809.051958940523</v>
       </c>
       <c r="K92" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L92" s="5">
         <f t="shared" si="3"/>
@@ -46103,7 +46066,7 @@
         <v>2565.793599251936</v>
       </c>
       <c r="K93" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L93" s="5">
         <f t="shared" si="3"/>
@@ -46148,7 +46111,7 @@
         <v>2427.5935992519362</v>
       </c>
       <c r="K94" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L94" s="5">
         <f t="shared" si="3"/>
@@ -46193,7 +46156,7 @@
         <v>2327.398599251936</v>
       </c>
       <c r="K95" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L95" s="5">
         <f t="shared" si="3"/>
@@ -46238,7 +46201,7 @@
         <v>3358.9857395066897</v>
       </c>
       <c r="K96" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L96" s="5">
         <f t="shared" si="3"/>
@@ -46283,7 +46246,7 @@
         <v>3328.8809589405228</v>
       </c>
       <c r="K97" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L97" s="5">
         <f t="shared" si="3"/>
@@ -46328,7 +46291,7 @@
         <v>3085.6225992519358</v>
       </c>
       <c r="K98" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L98" s="5">
         <f t="shared" si="3"/>
@@ -46373,7 +46336,7 @@
         <v>3045.4050819358285</v>
       </c>
       <c r="K99" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L99" s="5">
         <f t="shared" si="3"/>
@@ -46418,7 +46381,7 @@
         <v>3006.353599251936</v>
       </c>
       <c r="K100" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L100" s="5">
         <f t="shared" si="3"/>
@@ -46463,7 +46426,7 @@
         <v>2895.793599251936</v>
       </c>
       <c r="K101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L101" s="5">
         <f t="shared" si="3"/>
@@ -46572,10 +46535,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>34</v>
@@ -46584,13 +46547,13 @@
         <v>35</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -46598,7 +46561,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -46623,7 +46586,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="3">
         <v>0.5</v>
@@ -46648,7 +46611,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -47260,10 +47223,10 @@
         <v>54</v>
       </c>
       <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
         <v>69</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -47358,7 +47321,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" s="5">
         <f>'WFA 0-5 GIRLS'!L6</f>
@@ -53767,10 +53730,10 @@
         <v>54</v>
       </c>
       <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
         <v>69</v>
-      </c>
-      <c r="E1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -54112,19 +54075,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G1" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
+      <c r="G1" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -57440,23 +57403,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="H1" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
+      <c r="H1" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -61700,19 +61663,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="G1" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
+      <c r="G1" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>